<commit_message>
add time logs sprint 3
</commit_message>
<xml_diff>
--- a/organisation/Zeitaufzeichnung per Mitwirkender.xlsx
+++ b/organisation/Zeitaufzeichnung per Mitwirkender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffce2ed5387dd938/Dokumente/GitHub/cellarius/organisation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenop\Documents\!HTL2021\SYP\cellarius\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="8_{65C0D87D-C112-45DE-9386-F52D71E733B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19FD5BF3-3A65-45D8-827C-9B6F5751AB99}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C50AFBC-C480-4D55-BF0C-3C19883389B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18375" yWindow="1635" windowWidth="21870" windowHeight="16710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38910" yWindow="645" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,13 +754,21 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="12">
+        <v>1.0451388888888888</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1.1416666666666666</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1.0541666666666667</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.7729166666666667</v>
+      </c>
       <c r="F9" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.0138888888888893</v>
       </c>
       <c r="G9" s="18"/>
     </row>
@@ -825,23 +833,23 @@
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f>SUM(B5,B7,B6,B8,B9,B10,B11,B12,B13,B14)</f>
-        <v>2.2604166666666665</v>
+        <v>3.3055555555555554</v>
       </c>
       <c r="C15" s="17">
         <f>SUM(C5,C6,C7,C8,C9,C10,C11,C12,C13,C14)</f>
-        <v>3.1236111111111109</v>
+        <v>4.2652777777777775</v>
       </c>
       <c r="D15" s="17">
         <f>SUM(D5:D14)</f>
-        <v>2.3229166666666665</v>
+        <v>3.3770833333333332</v>
       </c>
       <c r="E15" s="17">
         <f>SUM(E5:E14)</f>
-        <v>2.2472222222222222</v>
+        <v>3.0201388888888889</v>
       </c>
       <c r="F15" s="21">
         <f t="shared" si="0"/>
-        <v>9.9541666666666657</v>
+        <v>13.968055555555555</v>
       </c>
       <c r="G15" s="18"/>
     </row>

</xml_diff>

<commit_message>
added Sprint 4 Zeitaufzeichung
changed Zeit der Mitwirkenden
</commit_message>
<xml_diff>
--- a/organisation/Zeitaufzeichnung per Mitwirkender.xlsx
+++ b/organisation/Zeitaufzeichnung per Mitwirkender.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zenop\Documents\!HTL2021\SYP\cellarius\organisation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhuiy\Documents\Github\cellarius\organisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C50AFBC-C480-4D55-BF0C-3C19883389B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F9FF5-FF3E-4C0B-8C99-8A8D43786565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38910" yWindow="645" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,6 +241,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,11 +779,21 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="22">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="D10" s="15">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0.34791666666666665</v>
+      </c>
       <c r="F10" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6909722222222221</v>
       </c>
       <c r="G10" s="18"/>
     </row>
@@ -833,23 +846,23 @@
       <c r="A15" s="16"/>
       <c r="B15" s="17">
         <f>SUM(B5,B7,B6,B8,B9,B10,B11,B12,B13,B14)</f>
-        <v>3.3055555555555554</v>
+        <v>3.6624999999999996</v>
       </c>
       <c r="C15" s="17">
         <f>SUM(C5,C6,C7,C8,C9,C10,C11,C12,C13,C14)</f>
-        <v>4.2652777777777775</v>
+        <v>4.7659722222222216</v>
       </c>
       <c r="D15" s="17">
         <f>SUM(D5:D14)</f>
-        <v>3.3770833333333332</v>
+        <v>3.8624999999999998</v>
       </c>
       <c r="E15" s="17">
         <f>SUM(E5:E14)</f>
-        <v>3.0201388888888889</v>
+        <v>3.3680555555555554</v>
       </c>
       <c r="F15" s="21">
         <f t="shared" si="0"/>
-        <v>13.968055555555555</v>
+        <v>15.659027777777778</v>
       </c>
       <c r="G15" s="18"/>
     </row>

</xml_diff>